<commit_message>
write with new sheet
</commit_message>
<xml_diff>
--- a/testdata/out_hostinfos.xlsx
+++ b/testdata/out_hostinfos.xlsx
@@ -7,7 +7,8 @@
     <ma:workbookView xWindow="5080" yWindow="1860" windowWidth="28240" windowHeight="17440"/>
   </ma:bookViews>
   <ma:sheets>
-    <ma:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <ma:sheet name="FirstSheet" sheetId="1" r:id="rId1"/>
+    <ma:sheet name="SecondSheet" sheetId="2" r:id="rId5"/>
   </ma:sheets>
   <ma:calcPr calcId="181029"/>
   <ma:extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<ma:sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" count="21" uniqueCount="21">
+<ma:sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" count="28" uniqueCount="28">
   <ma:si>
     <ma:t>主机名称</ma:t>
   </ma:si>
@@ -89,6 +90,27 @@
   </ma:si>
   <ma:si>
     <ma:t/>
+  </ma:si>
+  <ma:si>
+    <ma:t>主机名称</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>主机hostname</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>主机IP</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>主机负责人(rtx)</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>实例ID</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>服务器可用区</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>mb01第2页啦</ma:t>
   </ma:si>
 </ma:sst>
 </file>
@@ -584,4 +606,92 @@
   <ma:phoneticPr fontId="1" type="noConversion"/>
   <ma:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </ma:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<ma:worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+  <ma:dimension ref="A1:F4"/>
+  <ma:sheetData>
+    <ma:row r="1">
+      <ma:c r="A1" s="2" t="s">
+        <ma:v>21</ma:v>
+      </ma:c>
+      <ma:c r="B1" s="2" t="s">
+        <ma:v>22</ma:v>
+      </ma:c>
+      <ma:c r="C1" s="2" t="s">
+        <ma:v>23</ma:v>
+      </ma:c>
+      <ma:c r="D1" s="2" t="s">
+        <ma:v>24</ma:v>
+      </ma:c>
+      <ma:c r="E1" s="2" t="s">
+        <ma:v>25</ma:v>
+      </ma:c>
+      <ma:c r="F1" s="2" t="s">
+        <ma:v>26</ma:v>
+      </ma:c>
+    </ma:row>
+    <ma:row r="2">
+      <ma:c r="A2" s="1" t="s">
+        <ma:v>27</ma:v>
+      </ma:c>
+      <ma:c r="B2" s="1" t="s">
+        <ma:v>7</ma:v>
+      </ma:c>
+      <ma:c r="C2" s="1" t="s">
+        <ma:v>8</ma:v>
+      </ma:c>
+      <ma:c r="D2" s="1" t="s">
+        <ma:v>11</ma:v>
+      </ma:c>
+      <ma:c r="E2" s="1" t="s">
+        <ma:v>9</ma:v>
+      </ma:c>
+      <ma:c r="F2" s="1" t="s">
+        <ma:v>10</ma:v>
+      </ma:c>
+    </ma:row>
+    <ma:row r="3">
+      <ma:c r="A3" s="1" t="s">
+        <ma:v>12</ma:v>
+      </ma:c>
+      <ma:c r="B3" s="1" t="s">
+        <ma:v>13</ma:v>
+      </ma:c>
+      <ma:c r="C3" s="1" t="s">
+        <ma:v>14</ma:v>
+      </ma:c>
+      <ma:c r="D3" s="1" t="s">
+        <ma:v>11</ma:v>
+      </ma:c>
+      <ma:c r="E3" s="1" t="s">
+        <ma:v>15</ma:v>
+      </ma:c>
+      <ma:c r="F3" s="1" t="s">
+        <ma:v>10</ma:v>
+      </ma:c>
+    </ma:row>
+    <ma:row r="4">
+      <ma:c r="A4" s="1" t="s">
+        <ma:v>16</ma:v>
+      </ma:c>
+      <ma:c r="B4" s="1" t="s">
+        <ma:v>17</ma:v>
+      </ma:c>
+      <ma:c r="C4" s="1" t="s">
+        <ma:v>18</ma:v>
+      </ma:c>
+      <ma:c r="D4" s="1" t="s">
+        <ma:v>11</ma:v>
+      </ma:c>
+      <ma:c r="E4" s="1" t="s">
+        <ma:v>19</ma:v>
+      </ma:c>
+      <ma:c r="F4" s="1" t="s">
+        <ma:v>20</ma:v>
+      </ma:c>
+    </ma:row>
+  </ma:sheetData>
+</ma:worksheet>
 </file>
</xml_diff>